<commit_message>
Added some ERROR ACK information "When SIM_Card not present"
</commit_message>
<xml_diff>
--- a/sim800_cmds.xlsx
+++ b/sim800_cmds.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="181">
   <si>
     <t>Send SMS over SIM800 Module</t>
   </si>
@@ -398,9 +398,6 @@
     <t>\r\n&lt;Ccid data&gt;\r\n</t>
   </si>
   <si>
-    <t>Request Manufacturer Identification</t>
-  </si>
-  <si>
     <t>\r\n&lt;manufacturer&gt;\r\n</t>
   </si>
   <si>
@@ -431,9 +428,6 @@
     <t>AT+CGMI\n</t>
   </si>
   <si>
-    <t>Request Model Identification</t>
-  </si>
-  <si>
     <t>AT+CGMM\n</t>
   </si>
   <si>
@@ -444,9 +438,6 @@
 SIMCOM_SIM800
 OK
 </t>
-  </si>
-  <si>
-    <t>Request Product Serial Number Identification</t>
   </si>
   <si>
     <t>AT+CGSN\n</t>
@@ -816,6 +807,18 @@
   </si>
   <si>
     <t>Terminate HTTP Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\r\nERROR\r\n, Note errors occur if SIM is not inserted </t>
+  </si>
+  <si>
+    <t>Request Manufacturer Identification, This is GSM_related CMD, it's not depend on SIM</t>
+  </si>
+  <si>
+    <t>Request Model Identification, This is GSM_related CMD, it's not depend on SIM</t>
+  </si>
+  <si>
+    <t>Request Product Serial Number Identification (IMEI_No), This is GSM_related CMD, it's not depend on SIM</t>
   </si>
 </sst>
 </file>
@@ -929,7 +932,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1017,6 +1020,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1027,7 +1043,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1117,7 +1133,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1126,11 +1148,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1146,14 +1174,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1454,9 +1485,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1474,7 +1505,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
       <c r="A2" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>85</v>
@@ -1500,7 +1531,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B3" s="26">
         <v>1</v>
@@ -1524,7 +1555,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B4" s="25">
         <v>2</v>
@@ -1548,7 +1579,7 @@
     </row>
     <row r="5" spans="1:8" ht="60">
       <c r="A5" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B5" s="25">
         <v>3</v>
@@ -1571,289 +1602,289 @@
       <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1">
-      <c r="A6" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="33">
+      <c r="A6" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="35">
         <v>4</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="40">
         <v>2</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="H6" s="32" t="s">
-        <v>112</v>
+      <c r="H6" s="37" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="43"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" s="33">
+      <c r="A8" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="35">
         <v>5</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="40">
         <v>2</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G8" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>113</v>
+      <c r="G8" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="69" customHeight="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="43"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="34"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1">
-      <c r="A10" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B10" s="33">
+      <c r="A10" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="35">
         <v>6</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="40">
         <v>2</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>114</v>
+      <c r="G10" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="36.75" customHeight="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="43"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="32"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="75" customHeight="1">
-      <c r="A12" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="33">
+      <c r="A12" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="35">
         <v>7</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="40">
+        <v>2</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" s="43">
-        <v>2</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="H12" s="32" t="s">
-        <v>115</v>
+      <c r="H12" s="37" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="43"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="32"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:8" ht="75" customHeight="1">
-      <c r="A14" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B14" s="33">
+      <c r="A14" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="35">
         <v>8</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="40">
+        <v>2</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="G14" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="43">
-        <v>2</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="32" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="43"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="32"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:8" ht="75" customHeight="1">
-      <c r="A16" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B16" s="33">
+      <c r="A16" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="35">
         <v>9</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" s="40">
+        <v>2</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="E16" s="43">
-        <v>2</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="43"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="32"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
     </row>
     <row r="18" spans="1:8" ht="75" customHeight="1">
-      <c r="A18" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B18" s="33">
+      <c r="A18" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="35">
         <v>10</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="40">
+        <v>2</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="H18" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="43">
-        <v>2</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="43"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="32"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" ht="105">
       <c r="A20" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B20" s="25">
         <v>11</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E20" s="25">
         <v>1</v>
       </c>
-      <c r="F20" s="42" t="s">
-        <v>131</v>
+      <c r="F20" s="33" t="s">
+        <v>128</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>102</v>
@@ -1862,16 +1893,16 @@
     </row>
     <row r="21" spans="1:8" ht="75">
       <c r="A21" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B21" s="25">
         <v>12</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E21" s="25">
         <v>1</v>
@@ -1886,16 +1917,16 @@
     </row>
     <row r="22" spans="1:8" ht="75">
       <c r="A22" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B22" s="25">
         <v>13</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E22" s="25">
         <v>1</v>
@@ -1907,21 +1938,21 @@
         <v>102</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="151.5">
       <c r="A23" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B23" s="25">
         <v>14</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E23" s="25">
         <v>1</v>
@@ -1936,16 +1967,16 @@
     </row>
     <row r="24" spans="1:8" ht="45">
       <c r="A24" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B24" s="25">
         <v>15</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E24" s="25">
         <v>1</v>
@@ -1960,16 +1991,16 @@
     </row>
     <row r="25" spans="1:8" ht="30">
       <c r="A25" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B25" s="25">
         <v>16</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E25" s="25">
         <v>1</v>
@@ -1984,16 +2015,16 @@
     </row>
     <row r="26" spans="1:8" ht="30">
       <c r="A26" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B26" s="25">
         <v>17</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E26" s="25">
         <v>1</v>
@@ -2007,55 +2038,55 @@
       <c r="H26" s="21"/>
     </row>
     <row r="27" spans="1:8" ht="75" customHeight="1">
-      <c r="A27" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" s="33">
+      <c r="A27" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="35">
         <v>18</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="40">
+        <v>2</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="D27" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" s="43">
-        <v>2</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="G27" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="H27" s="32" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="43"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="40"/>
       <c r="F28" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G28" s="34"/>
-      <c r="H28" s="32"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
     </row>
     <row r="29" spans="1:8" ht="30">
       <c r="A29" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29" s="25">
         <v>19</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E29" s="25">
         <v>1</v>
@@ -2070,18 +2101,18 @@
     </row>
     <row r="30" spans="1:8" ht="30">
       <c r="A30" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B30" s="25">
         <v>20</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E30" s="44">
+        <v>148</v>
+      </c>
+      <c r="E30" s="34">
         <v>2</v>
       </c>
       <c r="F30" s="21" t="s">
@@ -2094,16 +2125,16 @@
     </row>
     <row r="31" spans="1:8" ht="79.5" thickBot="1">
       <c r="A31" s="29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B31" s="29">
         <v>21</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E31" s="29">
         <v>1</v>
@@ -2118,16 +2149,16 @@
     </row>
     <row r="33" spans="1:8" ht="45">
       <c r="A33" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33" s="25">
         <v>1</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E33" s="25">
         <v>1</v>
@@ -2142,16 +2173,16 @@
     </row>
     <row r="34" spans="1:8" ht="42.75">
       <c r="A34" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B34" s="25">
         <v>2</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E34" s="25">
         <v>1</v>
@@ -2166,16 +2197,16 @@
     </row>
     <row r="35" spans="1:8" ht="60">
       <c r="A35" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B35" s="25">
         <v>3</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E35" s="25">
         <v>1</v>
@@ -2190,16 +2221,16 @@
     </row>
     <row r="36" spans="1:8" ht="30">
       <c r="A36" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B36" s="25">
         <v>4</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E36" s="25">
         <v>1</v>
@@ -2213,141 +2244,141 @@
       <c r="H36" s="21"/>
     </row>
     <row r="37" spans="1:8" ht="78.75" customHeight="1">
-      <c r="A37" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B37" s="33">
+      <c r="A37" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="35">
         <v>5</v>
       </c>
-      <c r="C37" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="E37" s="43">
+      <c r="C37" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" s="40">
         <v>2</v>
       </c>
-      <c r="F37" s="42" t="s">
-        <v>168</v>
-      </c>
-      <c r="G37" s="34" t="s">
+      <c r="F37" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="G37" s="36" t="s">
         <v>102</v>
       </c>
       <c r="H37" s="21"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="43"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G38" s="34"/>
+      <c r="G38" s="36"/>
       <c r="H38" s="21"/>
     </row>
     <row r="39" spans="1:8" ht="91.5" customHeight="1">
-      <c r="A39" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" s="33">
+      <c r="A39" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="35">
         <v>6</v>
       </c>
-      <c r="C39" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="E39" s="43">
+      <c r="C39" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="40">
         <v>2</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G39" s="34" t="s">
+      <c r="G39" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="H39" s="32" t="s">
+      <c r="H39" s="37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="35"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
+    </row>
+    <row r="41" spans="1:8" ht="90" customHeight="1">
+      <c r="A41" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="35">
+        <v>7</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" s="40">
+        <v>3</v>
+      </c>
+      <c r="F41" s="21" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="42" t="s">
-        <v>171</v>
-      </c>
-      <c r="G40" s="34"/>
-      <c r="H40" s="32"/>
-    </row>
-    <row r="41" spans="1:8" ht="90" customHeight="1">
-      <c r="A41" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B41" s="33">
-        <v>7</v>
-      </c>
-      <c r="C41" s="32" t="s">
+      <c r="G41" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H41" s="37" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="D41" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="E41" s="43">
-        <v>3</v>
-      </c>
-      <c r="F41" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="G41" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="H41" s="32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="G42" s="34"/>
-      <c r="H42" s="32"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="43"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="40"/>
       <c r="F43" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="34"/>
-      <c r="H43" s="32"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1">
       <c r="A44" s="29" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B44" s="29">
         <v>8</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E44" s="29">
         <v>1</v>
@@ -2362,6 +2393,67 @@
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
@@ -2377,67 +2469,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="G41:G43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -2471,12 +2502,12 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="17" t="s">
@@ -2549,12 +2580,12 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="17" t="s">
@@ -2629,12 +2660,12 @@
       <c r="D21" s="20"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="17" t="s">
@@ -2720,14 +2751,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="9" t="s">
@@ -2808,34 +2839,34 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="90">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="37" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="36" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="75">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="32"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="45">
       <c r="A8" s="5" t="s">
@@ -2894,32 +2925,32 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="120">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="32" t="s">
+      <c r="B11" s="36"/>
+      <c r="C11" s="37" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="105">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="32"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="34"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="13" t="s">
@@ -2951,17 +2982,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>